<commit_message>
début des correction SEO
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Openclassrooms\Projets\Projet 4 Optimisez un site web existant\Projet 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37085C9-1B97-4A67-A2BB-AD0B343F2C92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2C30F3-E88A-48E6-B534-20388F38A990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3660" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau" sheetId="1" r:id="rId1"/>
-    <sheet name="Mots clés" sheetId="2" r:id="rId2"/>
+    <sheet name="PwP" sheetId="6" r:id="rId2"/>
+    <sheet name="Mesure" sheetId="5" r:id="rId3"/>
+    <sheet name="Axe" sheetId="3" r:id="rId4"/>
+    <sheet name="Lighthouse" sheetId="4" r:id="rId5"/>
+    <sheet name="Mots clés" sheetId="2" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tableau!$B$2:$K$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="132">
   <si>
     <t>Categorie</t>
   </si>
@@ -78,9 +85,6 @@
     <t>Localisation du problème</t>
   </si>
   <si>
-    <t>HTML ==&gt; HEAD</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://openclassrooms.com/fr/courses/5922626-optimiser-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques </t>
   </si>
   <si>
@@ -96,9 +100,6 @@
     <t>Il faut renseigner la langue en FR</t>
   </si>
   <si>
-    <t>HTML ==&gt; BODY</t>
-  </si>
-  <si>
     <t>Répétitions de mots clés dans la description de l'image</t>
   </si>
   <si>
@@ -111,9 +112,6 @@
     <t>Il n'y a pas de balise  "robots"</t>
   </si>
   <si>
-    <t>Ajouter une balise "robots "</t>
-  </si>
-  <si>
     <t>l'attribu "Content" n'est pas renseigné</t>
   </si>
   <si>
@@ -126,15 +124,9 @@
     <t>Il faut y inscrire : La chouette agence est une agence de web design qui aide les entreprises à devenir attractives et visibles sur internet</t>
   </si>
   <si>
-    <t>HTML ==&gt; FOOTER</t>
-  </si>
-  <si>
     <t xml:space="preserve">Il faut mettre des liens cohérent </t>
   </si>
   <si>
-    <t>Liens inutiles ou morts</t>
-  </si>
-  <si>
     <t>Agence web</t>
   </si>
   <si>
@@ -183,12 +175,6 @@
     <t>Remplacer les mots par logo de la chouette agence</t>
   </si>
   <si>
-    <t>Il n'y a pas de plan " Localisation "</t>
-  </si>
-  <si>
-    <t>Mots clés</t>
-  </si>
-  <si>
     <t>Région Lyonnaise</t>
   </si>
   <si>
@@ -201,37 +187,133 @@
     <t>Entreprises locales</t>
   </si>
   <si>
-    <r>
-      <t>Cette balise sert à expliquer le contenu de l'image aux moteurs de recherche et s'affiche quand les images ne peuvent être chargées. Elle sert aussi à décrire l'image pour les personnes malvoyantes. Il est donc conseillé de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>décrire correctement l'image et si possible</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>d'y ajouter le mot-clé. Cela étant, n'allez pas trop loin dans ce sens non plus. Ne surchargez pas les balises alt de mots clés dans le but de tromper Google. Il faut que les mots clés soient fidèles à l'image, et au reste du contenu de la page.</t>
-    </r>
+    <t>Remplacer les mots répétés par d'autres mots clés plus pertinants</t>
+  </si>
+  <si>
+    <t>Visible</t>
+  </si>
+  <si>
+    <t>Attractives</t>
+  </si>
+  <si>
+    <t>Agence design</t>
+  </si>
+  <si>
+    <t>La description de l image n'est pas correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si les mots clés ne sont pas cohérent ou répétés dans le site, le référencement ne se fera pas correctement </t>
+  </si>
+  <si>
+    <t>Supprimer la Div</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cacher des mots clés sur le site est une méthode qui est dépassée, elle est considérée comme du black-hat </t>
+  </si>
+  <si>
+    <t>Il ne faut pas cacher de mots sur le site</t>
+  </si>
+  <si>
+    <t>Page 2 : HTML ==&gt; ligne 5</t>
+  </si>
+  <si>
+    <t>Remettre les même mots clés que sur la première page</t>
+  </si>
+  <si>
+    <t>Page 2 : HTML ==&gt; ligne 39</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 40</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 42</t>
+  </si>
+  <si>
+    <t>HTML ==&gt; ligne 249</t>
+  </si>
+  <si>
+    <t>Page 2 : HTML ==&gt; ligne 38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette balise sert à expliquer la lague employée aux moteurs de recherche. </t>
+  </si>
+  <si>
+    <t>Il faut mettre des liens utiles, comme des liens partenaires ou les réseaux sociaux</t>
+  </si>
+  <si>
+    <t>Google suit les liens et indique si ils sont cohérents ou pas</t>
+  </si>
+  <si>
+    <t>Page 2 : HTML ==&gt; ligne 2</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 2</t>
+  </si>
+  <si>
+    <t>Page 2 : HTML ==&gt; ligne 21</t>
+  </si>
+  <si>
+    <t>Donner de la visibibilité</t>
+  </si>
+  <si>
+    <t>Devenir une entreprise attractive</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Mots Clés Trouvés</t>
+  </si>
+  <si>
+    <t>Mots Clés Vu Sur Le Site</t>
+  </si>
+  <si>
+    <t>Illustrations</t>
+  </si>
+  <si>
+    <t>Stratégie</t>
+  </si>
+  <si>
+    <t>Agence</t>
+  </si>
+  <si>
+    <t>Entreprise attractive</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Site web</t>
+  </si>
+  <si>
+    <t>Agence web basée à Lyon</t>
+  </si>
+  <si>
+    <t>Agence de web design</t>
+  </si>
+  <si>
+    <t>Graphiste</t>
+  </si>
+  <si>
+    <t>La Div class=keywords contient des mots clés cachés</t>
+  </si>
+  <si>
+    <t>Openclassrooms</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>Méta description :l'attribu "Content" n'est pas renseigné</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=FNXhHSn00js </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2nbHsBCYdp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UxIRq_bWE6I&amp;t=867s</t>
   </si>
   <si>
     <r>
@@ -240,7 +322,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -249,7 +331,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -259,7 +341,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -268,7 +350,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -277,26 +359,152 @@
     </r>
   </si>
   <si>
-    <t>Il faut ajouter la balise Robots dans la head pour que goolge index le contenu et suive les liens du site</t>
-  </si>
-  <si>
-    <t>Remplacer les mots répétés par d'autres mots clés plus pertinants</t>
+    <r>
+      <t>Cette balise sert à expliquer le contenu de l'image aux moteurs de recherche. Elle sert aussi à décrire l'image pour les personnes malvoyantes. Il est donc conseillé de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>décrire correctement l'image et si possible</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, d'y ajouter le mot-clé. Ne surchargez pas les balises alt de mots clés dans le but de tromper Google. Il faut que les mots clés soient fidèles à l'image, et au reste de la page.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.abondance.com/20110811-8990-validation-htmlw3c-et-positionnement-google-questionsreponses-avec-google-15.html </t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>https://www.seo.fr/definition/seo-definition</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 23</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 5</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 7</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 229</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 41</t>
+  </si>
+  <si>
+    <t>Page 2 : CSS ligne 679</t>
+  </si>
+  <si>
+    <t>Taille du paragraphe</t>
+  </si>
+  <si>
+    <t>Pour que le texte soit lisible la taille minimum doit être de 12px</t>
+  </si>
+  <si>
+    <t>La taille minimum doit être de 12px</t>
+  </si>
+  <si>
+    <t>Il faut changer 11 px par 12 px.</t>
+  </si>
+  <si>
+    <t>Liens qui retournent sur l'index</t>
+  </si>
+  <si>
+    <t>Ajouter une balise  Méta "robots "</t>
+  </si>
+  <si>
+    <t>Il faut ajouter la balise Méta "Robots" dans la head pour que goolge index le contenu et suive les liens du site</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Les images ne sont pas dans un format adapté</t>
+  </si>
+  <si>
+    <t>Les formats .bmp sont à convertir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les images sont trop lourdes à charger ce qui ralentit le chargement du site </t>
+  </si>
+  <si>
+    <t>Convertir les images au minimum en Jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 1 : HTML ==&gt; ligne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les h3 sont au dessus des h2 </t>
+  </si>
+  <si>
+    <t>Repecter la hierarchie des titres</t>
+  </si>
+  <si>
+    <t>La hierarchie entre les titres doit être respecter on doit avoir cette ordre H1 puis H2 puis H3 etc…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faire le changement dans le code </t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Page 1 : HTML ==&gt; ligne 698</t>
+  </si>
+  <si>
+    <t>Couleurs dans boutons pas assez contrasté</t>
+  </si>
+  <si>
+    <t>Boutons trop petit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il faut respecter le ratio de contraste </t>
+  </si>
+  <si>
+    <t>Pour que le texte soit lisible pour tous il faut respecter un ratio de contrast entre le texte et le background</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer les couleurs </t>
+  </si>
+  <si>
+    <t>Aggrandir le texte pour aggrandir le bouton</t>
+  </si>
+  <si>
+    <t>Il faut respecter la taille des élément pour que le texte à l'intérieur soit lisibles</t>
+  </si>
+  <si>
+    <t>3eme</t>
+  </si>
+  <si>
+    <t>Entreprise web design Lyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=U7FFbH8Bm5A </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -319,36 +527,9 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -360,14 +541,72 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="20"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF7030A0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,18 +616,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
-        <bgColor rgb="FF7030A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
@@ -407,11 +634,47 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -487,59 +750,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -552,7 +770,59 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -562,53 +832,65 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -617,87 +899,132 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,6 +1037,422 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>618705</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6C9831-79C2-4112-B90C-EDB538EDBE64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="381000"/>
+          <a:ext cx="3361905" cy="904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>577982</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>160957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DCC03A2-AB11-4ADA-AE89-44C13DBD4CFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531620" y="228600"/>
+          <a:ext cx="9104762" cy="7742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>814407</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>25620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2A4C5CB-A0E4-4A8D-9441-AC95647A8175}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1577340" y="8199120"/>
+          <a:ext cx="7466667" cy="8400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>17447</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ECA1B66-E89F-4A26-A309-AA76D3C08B8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="381000"/>
+          <a:ext cx="12819047" cy="4295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>750895</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>151619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B3B3360-8E49-4D66-A9F2-910BD554061C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="381000"/>
+          <a:ext cx="12638095" cy="6247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>646362</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>56524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B40826-611B-4808-B1C4-9BB6CBA51830}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="6858000"/>
+          <a:ext cx="10704762" cy="5009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>560648</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>56762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69B7A0C2-E264-4E20-A578-C7C819A26B7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="12001500"/>
+          <a:ext cx="10619048" cy="3104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>551124</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>170571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DFF4324-3C7D-4B59-8CB4-A46F7A9F30AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="15430500"/>
+          <a:ext cx="10609524" cy="7028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>198857</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>104119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{801A720F-4A9E-4B8E-8858-5EB6FCE71941}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="22669500"/>
+          <a:ext cx="9342857" cy="5247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,54 +1653,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1001"/>
+  <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="24.26953125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="28.26953125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="43.36328125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="59.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="104.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="28" width="10.54296875" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="11.1796875" style="1"/>
+    <col min="1" max="1" width="11.1796875" style="1"/>
+    <col min="2" max="2" width="3.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.7265625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="58.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.08984375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="49.36328125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="44.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.08984375" style="1" customWidth="1"/>
+    <col min="14" max="29" width="10.54296875" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="11.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="5.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:28" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="1:29" ht="5.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:29" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="H2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -973,409 +1730,751 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" s="3" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-    </row>
-    <row r="4" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="AC2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="C3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="D3" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="39"/>
+      <c r="J3" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="39"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="44"/>
+    </row>
+    <row r="5" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="39"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="44"/>
+    </row>
+    <row r="6" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="39"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="L6" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="M6" s="20"/>
+      <c r="N6" s="44"/>
+    </row>
+    <row r="7" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="39"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" s="20"/>
+      <c r="N7" s="44"/>
+    </row>
+    <row r="8" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="39"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="3">
+        <v>7</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="39"/>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="39"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:29" s="9" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G11" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="1:29" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="21" t="s">
+      <c r="I14" s="39"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>13</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="39"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="39"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="41"/>
+    </row>
+    <row r="17" spans="1:11" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="39"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="41"/>
+    </row>
+    <row r="18" spans="1:11" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="39"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="41"/>
+    </row>
+    <row r="19" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>2</v>
-      </c>
-      <c r="B5" s="36" t="s">
+      <c r="C19" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10" t="s">
+      <c r="D19" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="41"/>
+    </row>
+    <row r="20" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="3">
+        <v>18</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="3">
+        <v>19</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="16"/>
+    </row>
+    <row r="22" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="3">
         <v>20</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="174.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="C22" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="D22" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" s="1">
         <v>21</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>6</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>7</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>8</v>
-      </c>
-      <c r="B11" s="36" t="s">
+      <c r="C23" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>9</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>10</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>11</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
-        <v>12</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:28" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>13</v>
-      </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="24"/>
-    </row>
-    <row r="17" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>14</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>15</v>
-      </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>16</v>
-      </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>17</v>
-      </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>18</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="24"/>
-    </row>
-    <row r="22" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>19</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="1:8" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
-        <v>20</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D23" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K30" s="16"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="16"/>
+    </row>
+    <row r="43" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="16"/>
+    </row>
+    <row r="47" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="16"/>
+    </row>
+    <row r="48" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="16"/>
+    </row>
+    <row r="51" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K51" s="16"/>
+    </row>
+    <row r="52" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="16"/>
+    </row>
+    <row r="56" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="11:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2312,14 +3411,18 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="N3:N7"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{1CA8C525-D769-4CFB-B6F6-FF5BCA8B2B5C}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{8189B4E1-03FC-4E7E-A868-F38A600EF046}"/>
-    <hyperlink ref="H7" r:id="rId3" xr:uid="{B828AE91-E0EB-430E-B03E-8017D0246E52}"/>
-    <hyperlink ref="H8" r:id="rId4" xr:uid="{45048A0C-5F99-4555-975B-278370B57BBC}"/>
-    <hyperlink ref="H9" r:id="rId5" xr:uid="{4BE7BF16-6382-4AC8-89D2-985C5B49146D}"/>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{1CA8C525-D769-4CFB-B6F6-FF5BCA8B2B5C}"/>
+    <hyperlink ref="K5" r:id="rId2" xr:uid="{8189B4E1-03FC-4E7E-A868-F38A600EF046}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{746B5A91-6220-43EE-A1A8-52175A749B74}"/>
+    <hyperlink ref="M4" r:id="rId4" xr:uid="{B8B54B14-5266-48BF-B1B3-042867B6C84A}"/>
+    <hyperlink ref="L5" r:id="rId5" xr:uid="{DF786E02-4BA7-4E83-958D-0ACE13DB3BC6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId6"/>
@@ -2327,136 +3430,347 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF638C56-920C-4178-9F90-B1A3E4A64B48}">
-  <dimension ref="B2:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E7C15B-92B3-45C5-B763-7FA19259C10D}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FC4C9F-73DF-4F03-AEED-10921C53E21C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E59515-FFA0-4B06-BF05-F700257BB236}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B779294-F9FE-4506-801B-0B267EE99FBA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF638C56-920C-4178-9F90-B1A3E4A64B48}">
+  <dimension ref="C2:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
+    <col min="2" max="2" width="2.7265625" customWidth="1"/>
+    <col min="3" max="3" width="34.90625" customWidth="1"/>
+    <col min="4" max="4" width="3.36328125" customWidth="1"/>
+    <col min="5" max="5" width="35.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="3:6" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="10"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="3:6" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30"/>
-    </row>
-    <row r="4" spans="2:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="E24" s="45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="45" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="28"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="12"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="12"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="12"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="12"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="13" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout powerpoint et test SEO
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Openclassrooms\Projets\Projet 4 Optimisez un site web existant\Projet 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5FC22A-E6AB-4A5B-B6C1-7915200A1EA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF611F9-764D-441F-A034-BF006BCDF3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau" sheetId="1" r:id="rId1"/>
-    <sheet name="PwP" sheetId="6" r:id="rId2"/>
-    <sheet name="Mesure" sheetId="5" r:id="rId3"/>
-    <sheet name="Axe" sheetId="3" r:id="rId4"/>
-    <sheet name="Lighthouse" sheetId="4" r:id="rId5"/>
-    <sheet name="Mots clés" sheetId="2" r:id="rId6"/>
+    <sheet name="Feuil1" sheetId="7" r:id="rId2"/>
+    <sheet name="PwP" sheetId="6" r:id="rId3"/>
+    <sheet name="Mesure" sheetId="5" r:id="rId4"/>
+    <sheet name="Axe" sheetId="3" r:id="rId5"/>
+    <sheet name="Lighthouse" sheetId="4" r:id="rId6"/>
+    <sheet name="Mots clés" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tableau!$B$2:$K$2</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="143">
   <si>
     <t>Categorie</t>
   </si>
@@ -496,12 +497,45 @@
   <si>
     <t xml:space="preserve">https://www.youtube.com/watch?v=U7FFbH8Bm5A </t>
   </si>
+  <si>
+    <t>Lighthouse</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Mesure</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>Best practices</t>
+  </si>
+  <si>
+    <t>Avant</t>
+  </si>
+  <si>
+    <t>Après</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Infractions</t>
+  </si>
+  <si>
+    <t>Erreurs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -601,12 +635,32 @@
     </font>
     <font>
       <sz val="36"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +724,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -882,7 +954,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1004,9 +1076,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1019,6 +1088,48 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="13" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="14" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1523,13 +1634,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="1"/>
+    <col min="1" max="1" width="11.1796875" style="48"/>
     <col min="2" max="2" width="3.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.08984375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.1796875" style="4" bestFit="1" customWidth="1"/>
@@ -1578,11 +1689,11 @@
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
@@ -1601,8 +1712,8 @@
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>120</v>
+      <c r="A3" s="49">
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1626,7 +1737,7 @@
         <v>33</v>
       </c>
       <c r="I3" s="39"/>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="47" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="19" t="s">
@@ -1638,11 +1749,14 @@
       <c r="M3" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="47" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="49">
+        <v>9</v>
+      </c>
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -1665,7 +1779,7 @@
         <v>49</v>
       </c>
       <c r="I4" s="39"/>
-      <c r="J4" s="48"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="20" t="s">
         <v>16</v>
       </c>
@@ -1675,9 +1789,10 @@
       <c r="M4" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="48"/>
+      <c r="N4" s="47"/>
     </row>
     <row r="5" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -1700,7 +1815,7 @@
         <v>109</v>
       </c>
       <c r="I5" s="39"/>
-      <c r="J5" s="48"/>
+      <c r="J5" s="47"/>
       <c r="K5" s="20" t="s">
         <v>17</v>
       </c>
@@ -1710,11 +1825,11 @@
       <c r="M5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="N5" s="48"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
-        <v>120</v>
+      <c r="A6" s="49">
+        <v>3</v>
       </c>
       <c r="B6" s="3">
         <v>4</v>
@@ -1738,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="39"/>
-      <c r="J6" s="48"/>
+      <c r="J6" s="47"/>
       <c r="K6" s="20" t="s">
         <v>15</v>
       </c>
@@ -1746,9 +1861,12 @@
         <v>90</v>
       </c>
       <c r="M6" s="20"/>
-      <c r="N6" s="48"/>
+      <c r="N6" s="47"/>
     </row>
     <row r="7" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49">
+        <v>4</v>
+      </c>
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -1771,17 +1889,17 @@
         <v>66</v>
       </c>
       <c r="I7" s="39"/>
-      <c r="J7" s="48"/>
+      <c r="J7" s="47"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20" t="s">
         <v>91</v>
       </c>
       <c r="M7" s="20"/>
-      <c r="N7" s="48"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
-        <v>120</v>
+      <c r="A8" s="49">
+        <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>6</v>
@@ -1808,7 +1926,7 @@
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B9" s="3">
@@ -1836,7 +1954,7 @@
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B10" s="3">
@@ -1864,7 +1982,7 @@
       <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:29" s="9" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="3">
@@ -1892,6 +2010,9 @@
       <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:29" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49" t="s">
+        <v>120</v>
+      </c>
       <c r="B12" s="3">
         <v>10</v>
       </c>
@@ -1917,7 +2038,7 @@
       <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:29" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B13" s="3">
@@ -1945,7 +2066,7 @@
       <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B14" s="3">
@@ -1973,6 +2094,7 @@
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
       <c r="B15" s="3">
         <v>13</v>
       </c>
@@ -1999,8 +2121,8 @@
       <c r="K15" s="16"/>
     </row>
     <row r="16" spans="1:29" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
-        <v>120</v>
+      <c r="A16" s="49">
+        <v>5</v>
       </c>
       <c r="B16" s="3">
         <v>14</v>
@@ -2028,7 +2150,7 @@
       <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B17" s="3">
@@ -2057,8 +2179,8 @@
       <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" ht="139.94999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
-        <v>120</v>
+      <c r="A18" s="49">
+        <v>8</v>
       </c>
       <c r="B18" s="3">
         <v>16</v>
@@ -2086,8 +2208,8 @@
       <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
-        <v>120</v>
+      <c r="A19" s="49">
+        <v>7</v>
       </c>
       <c r="B19" s="3">
         <v>17</v>
@@ -2115,6 +2237,9 @@
       <c r="K19" s="41"/>
     </row>
     <row r="20" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49">
+        <v>8</v>
+      </c>
       <c r="B20" s="3">
         <v>18</v>
       </c>
@@ -2141,8 +2266,8 @@
       <c r="K20" s="16"/>
     </row>
     <row r="21" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
-        <v>120</v>
+      <c r="A21" s="49">
+        <v>6</v>
       </c>
       <c r="B21" s="3">
         <v>19</v>
@@ -2170,8 +2295,8 @@
       <c r="K21" s="16"/>
     </row>
     <row r="22" spans="1:11" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
-        <v>120</v>
+      <c r="A22" s="49">
+        <v>10</v>
       </c>
       <c r="B22" s="3">
         <v>20</v>
@@ -2199,7 +2324,7 @@
       <c r="K22" s="16"/>
     </row>
     <row r="23" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="49" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="1">
@@ -3298,6 +3423,257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2370B1E-DF8F-494B-A6D7-79E23734A64B}">
+  <dimension ref="E4:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="8.90625" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.36328125" customWidth="1"/>
+    <col min="10" max="10" width="8.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="5:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+    </row>
+    <row r="5" spans="5:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E5" s="53"/>
+      <c r="F5" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="53"/>
+    </row>
+    <row r="6" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E6" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="51">
+        <v>0.82</v>
+      </c>
+      <c r="G6" s="51">
+        <v>0.81</v>
+      </c>
+      <c r="H6" s="51">
+        <v>0.92</v>
+      </c>
+      <c r="I6" s="51">
+        <v>0.89</v>
+      </c>
+      <c r="J6" s="55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E7" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="52">
+        <v>0.98</v>
+      </c>
+      <c r="G7" s="52">
+        <v>1</v>
+      </c>
+      <c r="H7" s="52">
+        <v>0.92</v>
+      </c>
+      <c r="I7" s="52">
+        <v>1</v>
+      </c>
+      <c r="J7" s="55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E8" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="58">
+        <v>0.16</v>
+      </c>
+      <c r="G8" s="58">
+        <v>0.19</v>
+      </c>
+      <c r="H8" s="58">
+        <v>0</v>
+      </c>
+      <c r="I8" s="58">
+        <v>0.11</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="50"/>
+      <c r="J9" s="50"/>
+    </row>
+    <row r="10" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+    </row>
+    <row r="11" spans="5:10" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E11" s="53"/>
+      <c r="F11" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="53"/>
+    </row>
+    <row r="12" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E12" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="51">
+        <v>0.78</v>
+      </c>
+      <c r="G12" s="51">
+        <v>0.84</v>
+      </c>
+      <c r="H12" s="51">
+        <v>0.86</v>
+      </c>
+      <c r="I12" s="51">
+        <v>0.78</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E13" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="52">
+        <v>0.82</v>
+      </c>
+      <c r="G13" s="52">
+        <v>1</v>
+      </c>
+      <c r="H13" s="52">
+        <v>0.86</v>
+      </c>
+      <c r="I13" s="52">
+        <v>1</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E14" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="59">
+        <v>0.04</v>
+      </c>
+      <c r="G14" s="59">
+        <v>0.16</v>
+      </c>
+      <c r="H14" s="59">
+        <v>0</v>
+      </c>
+      <c r="I14" s="59">
+        <v>0.22</v>
+      </c>
+      <c r="J14" s="55" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="5:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="E16" s="56"/>
+      <c r="F16" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="57"/>
+    </row>
+    <row r="17" spans="5:7" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="E17" s="53"/>
+      <c r="F17" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="53"/>
+    </row>
+    <row r="18" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E18" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="60">
+        <v>35</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E19" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="61">
+        <v>0</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="E20" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="55">
+        <f>F19-F18</f>
+        <v>-35</v>
+      </c>
+      <c r="G20" s="55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E10:J10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E7C15B-92B3-45C5-B763-7FA19259C10D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3312,7 +3688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FC4C9F-73DF-4F03-AEED-10921C53E21C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3327,7 +3703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E59515-FFA0-4B06-BF05-F700257BB236}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3342,11 +3718,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B779294-F9FE-4506-801B-0B267EE99FBA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
@@ -3357,7 +3733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF638C56-920C-4178-9F90-B1A3E4A64B48}">
   <dimension ref="C2:F43"/>
   <sheetViews>
@@ -3417,10 +3793,10 @@
       <c r="C8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="44" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3436,7 +3812,7 @@
       <c r="C10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3528,7 +3904,7 @@
       <c r="C22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="43" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3552,7 +3928,7 @@
       <c r="C25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="43" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
recentrage et travail sur contraste
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1) (1).xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Openclassrooms\Projets\Projet 4 Optimisez un site web existant\Projet 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A435B34D-CD39-447A-945F-8FB7107D2F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36C14B5-992D-48E2-8E99-173913E6D60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tableau pwp" sheetId="8" r:id="rId1"/>
-    <sheet name="Tableau" sheetId="1" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="7" r:id="rId3"/>
+    <sheet name="Tableau" sheetId="1" r:id="rId1"/>
+    <sheet name="Tableau pwp" sheetId="8" r:id="rId2"/>
+    <sheet name="Perf~pwp" sheetId="7" r:id="rId3"/>
     <sheet name="Mots clés" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tableau!$B$2:$J$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tableau pwp'!$B$2:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tableau!$B$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tableau pwp'!$B$2:$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="145">
   <si>
     <t>Categorie</t>
   </si>
@@ -531,12 +531,15 @@
   <si>
     <t>Répétitions de mots clés sans cohérence</t>
   </si>
+  <si>
+    <t>Remplacer les mots clé par logo de la chouette agence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -686,13 +689,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -774,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -912,22 +908,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1046,18 +1033,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1089,13 +1064,16 @@
     <xf numFmtId="0" fontId="21" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1314,1382 +1292,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B4401D-754D-425B-8CDD-8139CD83EC6C}">
-  <dimension ref="A1:X993"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.1796875" style="19"/>
-    <col min="2" max="2" width="21.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="63.08984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="41.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="44.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="46.08984375" style="1" customWidth="1"/>
-    <col min="9" max="24" width="10.54296875" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.1796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="5.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:24" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50">
-        <v>1</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="45.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50">
-        <v>2</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="I4" s="55"/>
-    </row>
-    <row r="5" spans="1:24" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50">
-        <v>3</v>
-      </c>
-      <c r="B5" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" s="55"/>
-    </row>
-    <row r="6" spans="1:24" ht="45.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50">
-        <v>4</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="55"/>
-    </row>
-    <row r="7" spans="1:24" ht="30.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50">
-        <v>5</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" s="56"/>
-      <c r="I7" s="55"/>
-    </row>
-    <row r="8" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="50">
-        <v>6</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="50">
-        <v>7</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="50">
-        <v>8</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:24" s="5" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="50">
-        <v>9</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="50">
-        <v>10</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:24" s="31" customFormat="1" ht="28.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50">
-        <v>11</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="50">
-        <v>12</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="18"/>
-    </row>
-    <row r="15" spans="1:24" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="50">
-        <v>13</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:24" ht="28.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50">
-        <v>14</v>
-      </c>
-      <c r="B16" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="28.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="50">
-        <v>15</v>
-      </c>
-      <c r="B17" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F47" s="8"/>
-    </row>
-    <row r="48" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F48" s="8"/>
-    </row>
-    <row r="49" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F49" s="8"/>
-    </row>
-    <row r="50" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="I3:I7"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{F7C72561-7DA8-4BDD-ACF2-BB728C1583CB}"/>
-    <hyperlink ref="F5" r:id="rId2" xr:uid="{4368AF05-A610-4835-8F97-941E0B0C6D0A}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{1F8BAFF0-9CC7-4FF1-B8FB-BD66C776B7C5}"/>
-    <hyperlink ref="H4" r:id="rId4" xr:uid="{5D1EB902-5700-44F1-8800-D9BDF53AD5E8}"/>
-    <hyperlink ref="G5" r:id="rId5" xr:uid="{E7463612-8B07-4AE3-941D-526155CBA690}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2722,31 +1329,31 @@
       <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:28" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="40" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -2765,9 +1372,7 @@
       <c r="AB2" s="2"/>
     </row>
     <row r="3" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45">
-        <v>1</v>
-      </c>
+      <c r="A3" s="41"/>
       <c r="B3" s="33" t="s">
         <v>10</v>
       </c>
@@ -2787,7 +1392,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="17"/>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="53" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="11" t="s">
@@ -2799,14 +1404,12 @@
       <c r="L3" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="53" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="45">
-        <v>2</v>
-      </c>
+      <c r="A4" s="41"/>
       <c r="B4" s="33" t="s">
         <v>10</v>
       </c>
@@ -2826,7 +1429,7 @@
         <v>52</v>
       </c>
       <c r="H4" s="17"/>
-      <c r="I4" s="42"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
@@ -2836,10 +1439,10 @@
       <c r="L4" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="M4" s="42"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="5" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45">
+      <c r="A5" s="41">
         <v>3</v>
       </c>
       <c r="B5" s="33" t="s">
@@ -2861,7 +1464,7 @@
         <v>26</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="42"/>
+      <c r="I5" s="53"/>
       <c r="J5" s="12" t="s">
         <v>16</v>
       </c>
@@ -2871,10 +1474,10 @@
       <c r="L5" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="42"/>
+      <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:28" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="45">
+      <c r="A6" s="41">
         <v>4</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -2896,7 +1499,7 @@
         <v>63</v>
       </c>
       <c r="H6" s="17"/>
-      <c r="I6" s="42"/>
+      <c r="I6" s="53"/>
       <c r="J6" s="12" t="s">
         <v>14</v>
       </c>
@@ -2904,10 +1507,10 @@
         <v>85</v>
       </c>
       <c r="L6" s="12"/>
-      <c r="M6" s="42"/>
+      <c r="M6" s="53"/>
     </row>
     <row r="7" spans="1:28" ht="74.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45">
+      <c r="A7" s="41">
         <v>5</v>
       </c>
       <c r="B7" s="35" t="s">
@@ -2929,16 +1532,16 @@
         <v>43</v>
       </c>
       <c r="H7" s="17"/>
-      <c r="I7" s="42"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12" t="s">
         <v>86</v>
       </c>
       <c r="L7" s="12"/>
-      <c r="M7" s="42"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
+      <c r="A8" s="41">
         <v>6</v>
       </c>
       <c r="B8" s="33" t="s">
@@ -2963,7 +1566,7 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45">
+      <c r="A9" s="41">
         <v>7</v>
       </c>
       <c r="B9" s="35" t="s">
@@ -2988,7 +1591,7 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
+      <c r="A10" s="41">
         <v>8</v>
       </c>
       <c r="B10" s="35" t="s">
@@ -3013,7 +1616,7 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:28" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
+      <c r="A11" s="41">
         <v>8</v>
       </c>
       <c r="B11" s="33" t="s">
@@ -3038,7 +1641,7 @@
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:28" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
+      <c r="A12" s="41">
         <v>9</v>
       </c>
       <c r="B12" s="35" t="s">
@@ -3063,7 +1666,7 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:28" s="31" customFormat="1" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46">
+      <c r="A13" s="42">
         <v>10</v>
       </c>
       <c r="B13" s="36" t="s">
@@ -3089,7 +1692,7 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:28" s="31" customFormat="1" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="42">
         <v>11</v>
       </c>
       <c r="B14" s="33" t="s">
@@ -3115,7 +1718,7 @@
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:28" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
+      <c r="A15" s="41">
         <v>12</v>
       </c>
       <c r="B15" s="33" t="s">
@@ -3141,7 +1744,7 @@
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:28" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
+      <c r="A16" s="41">
         <v>13</v>
       </c>
       <c r="B16" s="33" t="s">
@@ -3167,7 +1770,7 @@
       <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="45">
+      <c r="A17" s="41">
         <v>14</v>
       </c>
       <c r="B17" s="33" t="s">
@@ -3193,7 +1796,7 @@
       <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" ht="52.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="A18" s="41">
         <v>15</v>
       </c>
       <c r="B18" s="33" t="s">
@@ -3219,7 +1822,7 @@
       <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
+      <c r="A19" s="41">
         <v>16</v>
       </c>
       <c r="B19" s="35" t="s">
@@ -3245,7 +1848,7 @@
       <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="45">
+      <c r="A20" s="41">
         <v>17</v>
       </c>
       <c r="B20" s="35" t="s">
@@ -3271,7 +1874,7 @@
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="45">
+      <c r="A21" s="41">
         <v>18</v>
       </c>
       <c r="B21" s="35" t="s">
@@ -3297,7 +1900,7 @@
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="45">
+      <c r="A22" s="41">
         <v>19</v>
       </c>
       <c r="B22" s="33" t="s">
@@ -3323,7 +1926,7 @@
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="45" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45">
+      <c r="A23" s="41">
         <v>20</v>
       </c>
       <c r="B23" s="36" t="s">
@@ -3342,14 +1945,14 @@
         <v>88</v>
       </c>
       <c r="G23" s="39" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="44.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="45">
+      <c r="A24" s="41">
         <v>21</v>
       </c>
       <c r="B24" s="33" t="s">
@@ -4441,12 +3044,1224 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B4401D-754D-425B-8CDD-8139CD83EC6C}">
+  <dimension ref="A1:Q993"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" style="19"/>
+    <col min="2" max="2" width="21.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="63.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" style="3" customWidth="1"/>
+    <col min="5" max="17" width="10.54296875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="5.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:17" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>1</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>2</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>3</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="46">
+        <v>4</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>5</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="17"/>
+    </row>
+    <row r="8" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="46">
+        <v>6</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="46">
+        <v>7</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
+        <v>8</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" s="5" customFormat="1" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
+        <v>9</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
+        <v>10</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" s="31" customFormat="1" ht="28.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="46">
+        <v>11</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="46">
+        <v>12</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="1:17" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="46">
+        <v>13</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:17" ht="28.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46">
+        <v>14</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="46">
+        <v>15</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2370B1E-DF8F-494B-A6D7-79E23734A64B}">
   <dimension ref="E4:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4460,14 +4275,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="5:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
     </row>
     <row r="5" spans="5:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="E5" s="23"/>
@@ -4550,14 +4365,14 @@
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="5:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
     </row>
     <row r="11" spans="5:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="E11" s="23"/>
@@ -4710,202 +4525,202 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" ht="6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="43" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="43" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="43" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="43" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="43" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="47"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="13" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="14" spans="1:5" ht="8.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="47"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="43" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="43" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>